<commit_message>
Small adjustments, adding links to data
</commit_message>
<xml_diff>
--- a/src/dbBuilders/featurestalents.xlsx
+++ b/src/dbBuilders/featurestalents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\projectflimflam\src\dbBuilders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39B5F58-6356-421A-AD7A-F8DB2BC34153}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B46669-0540-42EF-AFAE-8E99A3934699}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="3540" windowWidth="17970" windowHeight="15195" xr2:uid="{2343F6F3-6E68-4900-B14C-E2C7C179D031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2343F6F3-6E68-4900-B14C-E2C7C179D031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -259,6 +259,42 @@
   </si>
   <si>
     <t>Clerics can cast their spells as rituals. (See Rituals.)</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Barbarian_Rage</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Barbaric_Cleave</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Building_Frenzy</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Slayer</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Strongheart</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Unstoppable</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Whirlwind</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Natural_Will</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Violence</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Ancestral_Warband</t>
+  </si>
+  <si>
+    <t>https://www.13thagesrd.com/classes/barbarian/#Relentless</t>
   </si>
 </sst>
 </file>
@@ -623,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066F239D-4F93-4ADB-9816-9761CBB30DA8}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,10 +670,11 @@
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="105.5703125" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -662,8 +699,11 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -688,8 +728,11 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -715,8 +758,11 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
@@ -742,8 +788,11 @@
       <c r="H4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -769,8 +818,11 @@
       <c r="H5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -796,8 +848,11 @@
       <c r="H6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -823,8 +878,11 @@
       <c r="H7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -850,8 +908,11 @@
       <c r="H8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -877,8 +938,11 @@
       <c r="H9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -904,8 +968,11 @@
       <c r="H10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -931,8 +998,11 @@
       <c r="H11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -958,8 +1028,11 @@
       <c r="H12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -986,7 +1059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1013,7 +1086,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1040,7 +1113,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>

</xml_diff>